<commit_message>
Initial commit: Upload all server files
</commit_message>
<xml_diff>
--- a/batch/all_videos.xlsx
+++ b/batch/all_videos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,41 +503,41 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>C-sitwuRdlM</t>
+          <t>DOmh6EPMeCY</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>More Day Drinking with Sabrina Carpenter</t>
+          <t>"What Would You Do?" — Bill O'Reilly Dissects Kamala Harris' Reaction to Venezuela</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>While day drinking in New York City, Seth and Sabrina Carpenter make drinks based on Sabrina's songs and play drinking games that involve identifying famous men based on their childhood photos and challenging each other to turn random phrases into innuendos.</t>
+          <t>Subscribe to never miss an episode of No Spin News with Bill O'Reilly: https://www.youtube.com/channel/UC4OvD2yIbofl9l4dIlqSNMw</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2025-12-22T23:00:30Z</t>
+          <t>2026-01-05T22:40:19Z</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>438</v>
+        <v>135</v>
       </c>
       <c r="F2" t="n">
-        <v>428433</v>
+        <v>31521</v>
       </c>
       <c r="G2" t="n">
-        <v>537</v>
+        <v>163</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Late Night with Seth Meyers</t>
+          <t>Bill O'Reilly</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=C-sitwuRdlM</t>
+          <t>https://www.youtube.com/watch?v=DOmh6EPMeCY</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -558,32 +558,32 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>77CKm5W3uJo</t>
+          <t>5OJrS2xAoBQ</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Bill O'Reilly on Abraham Lincoln, Jesus, and Christmas</t>
+          <t>Bill O'Reilly &amp; Tim Graham on Internet Bias</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Bill talks about some of the history of Christmas you may not know about.</t>
+          <t>Newsbusters.org and Media Research Center's Tim Graham joins Bill to discuss liberal bias on the internet.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2025-12-24T12:00:23Z</t>
+          <t>2026-01-04T13:00:18Z</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>363</v>
+        <v>600</v>
       </c>
       <c r="F3" t="n">
-        <v>27984</v>
+        <v>18106</v>
       </c>
       <c r="G3" t="n">
-        <v>128</v>
+        <v>74</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -592,7 +592,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=77CKm5W3uJo</t>
+          <t>https://www.youtube.com/watch?v=5OJrS2xAoBQ</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -613,41 +613,41 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>64_o8CY4lsc</t>
+          <t>s6W05lQNFuk</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Bill O'Reilly on Christmas in Levittown, New York</t>
+          <t>He just accidentally EXPOSED Trump’s incompetence</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Bill O'Reilly reminisces on Christmas in Levittown, New York.</t>
+          <t>-- Marco Rubio tells Kristen Welker the United States is running Venezuela but cannot explain elections, governance, or the legal rationale in real time</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2025-12-20T21:38:34Z</t>
+          <t>2026-01-06T03:30:48Z</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>392</v>
+        <v>417</v>
       </c>
       <c r="F4" t="n">
-        <v>77007</v>
+        <v>22171</v>
       </c>
       <c r="G4" t="n">
-        <v>353</v>
+        <v>277</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Bill O'Reilly</t>
+          <t>David Pakman Show</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=64_o8CY4lsc</t>
+          <t>https://www.youtube.com/watch?v=s6W05lQNFuk</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -668,41 +668,41 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>khNQnR_JRTk</t>
+          <t>UUrO5jWKlGU</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Bill O'Reilly on the Latest Example of Activist Judges Enabling Crime</t>
+          <t>Trump is about to get REJECTED</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Bill argues that today’s legal system does not want to punish criminals, pointing to the judges in a recent Tennessee case as an example.</t>
+          <t>-- Donald Trump bets the Maduro seizure will unlock Venezuela’s oil, but allies, businesses, and markets resist a plan with no clear political transition</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2025-12-19T19:00:53Z</t>
+          <t>2026-01-06T00:45:04Z</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>429</v>
+        <v>343</v>
       </c>
       <c r="F5" t="n">
-        <v>145267</v>
+        <v>155550</v>
       </c>
       <c r="G5" t="n">
-        <v>507</v>
+        <v>1166</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Bill O'Reilly</t>
+          <t>David Pakman Show</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=khNQnR_JRTk</t>
+          <t>https://www.youtube.com/watch?v=UUrO5jWKlGU</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -723,32 +723,32 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>jFVolN0zlfw</t>
+          <t>NJri0m1Uwiw</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>You’re not dumb enough to fall for this, right?</t>
+          <t>OH NO: Trump has NO IDEA what’s going on</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>-- Interior Secretary Doug Burgum misleads audiences about wind energy reliability and national security while ignoring grid diversification, storage technology, and documented fossil fuel failures</t>
+          <t>-- Donald Trump admits he did not brief Congress yet says he spoke with oil companies and calls the Maduro seizure a kidnapping</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2025-12-28T00:45:04Z</t>
+          <t>2026-01-05T23:30:16Z</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>459</v>
+        <v>480</v>
       </c>
       <c r="F6" t="n">
-        <v>68037</v>
+        <v>57721</v>
       </c>
       <c r="G6" t="n">
-        <v>630</v>
+        <v>593</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -757,7 +757,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=jFVolN0zlfw</t>
+          <t>https://www.youtube.com/watch?v=NJri0m1Uwiw</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -778,32 +778,32 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ZemdvNCV0oI</t>
+          <t>w0fPlxAgKaQ</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Trump PANICS over DISASTER Epstein files</t>
+          <t>BOMBSHELL report: Trump health DETERIORATING QUICKLY</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>-- The Trump Justice Department releases thousands of Epstein documents while simultaneously warning the public that claims about Donald Trump are false, signaling political damage control</t>
+          <t>-- The Wall Street Journal reports Donald Trump shows visible signs of decline, disputes doctors, and mislabels a CT scan as an MRI while aides manage optics</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2025-12-27T22:15:02Z</t>
+          <t>2026-01-05T22:15:05Z</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>410</v>
+        <v>522</v>
       </c>
       <c r="F7" t="n">
-        <v>185545</v>
+        <v>232344</v>
       </c>
       <c r="G7" t="n">
-        <v>1153</v>
+        <v>1882</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -812,7 +812,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=ZemdvNCV0oI</t>
+          <t>https://www.youtube.com/watch?v=w0fPlxAgKaQ</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -833,32 +833,32 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>b1hosqDv4Bw</t>
+          <t>qYk-K8lhZHc</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>They are threatening her with PRISON</t>
+          <t>Trump invaded Venezuela because Maduro was dancing</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>-- Lawmakers from both parties move toward contempt proceedings against Attorney General Pam Bondi for defying the Epstein Files Transparency Act and removing mandated documents</t>
+          <t>-- Reporting says Donald Trump escalates to military action after Nicolás Maduro dances on Venezuelan state television and aides treat it as personal mockery</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2025-12-27T21:00:41Z</t>
+          <t>2026-01-05T21:01:04Z</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>255</v>
+        <v>341</v>
       </c>
       <c r="F8" t="n">
-        <v>263768</v>
+        <v>44235</v>
       </c>
       <c r="G8" t="n">
-        <v>1872</v>
+        <v>745</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -867,7 +867,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=b1hosqDv4Bw</t>
+          <t>https://www.youtube.com/watch?v=qYk-K8lhZHc</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -888,32 +888,32 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>KGZ7_fJWcCE</t>
+          <t>ldXNWL_w-Ao</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Trump officials revive the dumbest anti-wind talking point #shorts</t>
+          <t>Is Trump even aware of what he just did?</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Become a Member: https://www.davidpakman.com/membership</t>
+          <t>-- Donald Trump gives rambling, conflicting answers about Venezuela, oil, and military escalation that raise questions about his decision making</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2025-12-27T14:00:35Z</t>
+          <t>2026-01-05T19:45:03Z</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>180</v>
+        <v>487</v>
       </c>
       <c r="F9" t="n">
-        <v>30829</v>
+        <v>307391</v>
       </c>
       <c r="G9" t="n">
-        <v>128</v>
+        <v>3225</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -922,7 +922,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=KGZ7_fJWcCE</t>
+          <t>https://www.youtube.com/watch?v=ldXNWL_w-Ao</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -943,41 +943,41 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>8tPPmbkX7fo</t>
+          <t>sy8ncMFEPdE</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Trump FREAKS OUT over Epstein in Christmas night MELTDOWN</t>
+          <t>Trump invaded Venezuela… because Maduro danced? #shorts</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>BREAKING #news - Trump complains about Epstein in Christmas night message</t>
+          <t>Become a Member: https://www.davidpakman.com/membership</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2025-12-26T02:04:16Z</t>
+          <t>2026-01-05T17:21:46Z</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>499</v>
+        <v>148</v>
       </c>
       <c r="F10" t="n">
-        <v>800034</v>
+        <v>152418</v>
       </c>
       <c r="G10" t="n">
-        <v>3980</v>
+        <v>1051</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Brian Tyler Cohen</t>
+          <t>David Pakman Show</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=8tPPmbkX7fo</t>
+          <t>https://www.youtube.com/watch?v=sy8ncMFEPdE</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -998,32 +998,32 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ATbs9E1KIuo</t>
+          <t>1BU_O3mQkKI</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Trump issues CREEPY Christmas message to young girl</t>
+          <t>Trump gets BRUTALLY EXPOSED amid Venezuela invasion | Another Day</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>BREAKING #news - Trump fumbles in Christmas calls to children</t>
+          <t xml:space="preserve">Trump gets unwelcome SURPRISE amid Venezuela invasion | Another Day </t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2025-12-25T04:08:32Z</t>
+          <t>2026-01-06T05:00:02Z</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>483</v>
+        <v>511</v>
       </c>
       <c r="F11" t="n">
-        <v>304130</v>
+        <v>45972</v>
       </c>
       <c r="G11" t="n">
-        <v>3215</v>
+        <v>454</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -1032,7 +1032,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=ATbs9E1KIuo</t>
+          <t>https://www.youtube.com/watch?v=1BU_O3mQkKI</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1053,41 +1053,41 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>JwsMjulZTas</t>
+          <t>r81CCwvN5K8</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>More countries prefer to borrow RMB instead of US dollars:  lower costs, bigger investments</t>
+          <t>Trump makes GRAVE MISTAKE with Venezuela invasion</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>More countries are converting their USD-denominated loans into RMB debt.</t>
+          <t>INTERVIEW: Biden’s deputy national security adviser Jon Finer on Trump’s Venezuela invasion</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2025-12-26T12:51:29Z</t>
+          <t>2026-01-06T02:59:07Z</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>435</v>
+        <v>692</v>
       </c>
       <c r="F12" t="n">
-        <v>58036</v>
+        <v>170989</v>
       </c>
       <c r="G12" t="n">
-        <v>621</v>
+        <v>1471</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Inside China Business</t>
+          <t>Brian Tyler Cohen</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=JwsMjulZTas</t>
+          <t>https://www.youtube.com/watch?v=r81CCwvN5K8</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1108,41 +1108,41 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>7X5NV_6rtq0</t>
+          <t>26fV3ovDlF8</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>China quietly takes over another trillion dollar industry</t>
+          <t>Mark Kelly drops BOMB on Pete Hegseth for trying to downgrade his rank</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Remote sensing is an earth science that is critical for infrastructure, oil and gas, heavy construction, forestry, and urban planning.   Remote sensing is also vital in military applications.</t>
+          <t>INTERVIEW: Sen. Mark Kelly reacts to Pete Hegseth’s attempt to downrank him</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2025-12-25T15:41:07Z</t>
+          <t>2026-01-06T00:59:05Z</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>441</v>
+        <v>621</v>
       </c>
       <c r="F13" t="n">
-        <v>118698</v>
+        <v>257354</v>
       </c>
       <c r="G13" t="n">
-        <v>824</v>
+        <v>1585</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Inside China Business</t>
+          <t>Brian Tyler Cohen</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=7X5NV_6rtq0</t>
+          <t>https://www.youtube.com/watch?v=26fV3ovDlF8</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -1163,32 +1163,32 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>5zTU_ZbJ3JE</t>
+          <t>BhoTv296dp8</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>The best way to make money in China:  stay away</t>
+          <t>How Huawei is winning the race for global 5G telecom dominance:  US firms didn't even show up</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>The world's richest brands are struggling in China, as domestic firms are more innovative, faster to market with new products, and aggressively cut prices to grow market share.</t>
+          <t>Half the world's population now relies on telecommunications powered by Huawei and other Chinese companies.</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2025-12-21T02:26:08Z</t>
+          <t>2026-01-06T02:14:01Z</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>484</v>
+        <v>351</v>
       </c>
       <c r="F14" t="n">
-        <v>119191</v>
+        <v>19760</v>
       </c>
       <c r="G14" t="n">
-        <v>1131</v>
+        <v>308</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=5zTU_ZbJ3JE</t>
+          <t>https://www.youtube.com/watch?v=BhoTv296dp8</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -1218,32 +1218,32 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>OKQMER75Vms</t>
+          <t>6vw4hKAzo0k</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>China wants to mass-produce space rockets like cars</t>
+          <t>Revolutionary generator transforms Chinese factories into power plants</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve">China is moving to a lean manufacturing model to mass produce space vehicles. </t>
+          <t>Chinese engineers deployed the world's first commercially viable sCO2 power generators, at a steel mill in Guizhou.</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2025-12-16T14:06:28Z</t>
+          <t>2026-01-05T14:51:18Z</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>354</v>
+        <v>281</v>
       </c>
       <c r="F15" t="n">
-        <v>71388</v>
+        <v>57164</v>
       </c>
       <c r="G15" t="n">
-        <v>615</v>
+        <v>738</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -1252,7 +1252,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=OKQMER75Vms</t>
+          <t>https://www.youtube.com/watch?v=6vw4hKAzo0k</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -1273,32 +1273,32 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>O7L1C1_e88c</t>
+          <t>Bq1PDD5SWS0</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>China's export juggernaut:  low prices and booming trade to rest of world, while Americans buy less</t>
+          <t>China plus Russia plus Iran plus North Korea: builds 70% of the world's warships</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>High tariffs in the United States resulted in a sharp $38 billion reduction in Chinese imports in the 3rd quarter, compared to the same period in 2024.</t>
+          <t>China's dominance in commercial shipbuilding is hugely advantageous to the Chinese Navy, which is now the largest in the world.</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2025-12-04T15:43:44Z</t>
+          <t>2026-01-04T12:09:37Z</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>464</v>
+        <v>494</v>
       </c>
       <c r="F16" t="n">
-        <v>62146</v>
+        <v>59070</v>
       </c>
       <c r="G16" t="n">
-        <v>653</v>
+        <v>749</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -1307,7 +1307,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=O7L1C1_e88c</t>
+          <t>https://www.youtube.com/watch?v=Bq1PDD5SWS0</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1324,6 +1324,666 @@
         <v>0</v>
       </c>
       <c r="M16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>qzue-WRW5MY</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>China and Russia in the Arctic have NATO and Europe worried</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>NATO and European officials are deeply concerned, as China and Russia enjoy scientific, commercial, and military breakthroughs across the Arctic region.</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2026-01-03T13:33:29Z</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>513</v>
+      </c>
+      <c r="F17" t="n">
+        <v>40613</v>
+      </c>
+      <c r="G17" t="n">
+        <v>554</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Inside China Business</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=qzue-WRW5MY</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>简体中文</t>
+        </is>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>azAGvW91wss</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Aluminum prices soar on Trump tariffs, global shortages, and China supply chain moves</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>American buyers of aluminum are paying record spreads over global benchmarks, amid Trump's 50% tariffs and worldwide shortages of industrial metals.</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2026-01-02T13:46:45Z</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>409</v>
+      </c>
+      <c r="F18" t="n">
+        <v>59704</v>
+      </c>
+      <c r="G18" t="n">
+        <v>481</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Inside China Business</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=azAGvW91wss</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>简体中文</t>
+        </is>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>t0a6IDHRq1o</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Nvidia is in big trouble, as Huawei rolls out 5G and AI across the world</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nvidia faces severe challenges, as China's monopolies on gallium allow its telecom providers to build low-cost 5G telecom across the world.  </t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2025-12-30T11:00:55Z</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>498</v>
+      </c>
+      <c r="F19" t="n">
+        <v>107288</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1219</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Inside China Business</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=t0a6IDHRq1o</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>简体中文</t>
+        </is>
+      </c>
+      <c r="L19" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>qo8QnxqF92Y</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>AI is revolutionizing Chinese coal production, and blowing up labor models everywhere else</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Coal prices are in steep decline across the world, and that should translate to collapsing profitability for coal miners.</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2025-12-29T13:26:55Z</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>360</v>
+      </c>
+      <c r="F20" t="n">
+        <v>63274</v>
+      </c>
+      <c r="G20" t="n">
+        <v>586</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Inside China Business</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=qo8QnxqF92Y</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>简体中文</t>
+        </is>
+      </c>
+      <c r="L20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>xged_Pzo35Q</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Trump VISIBLY STUNS Lindsey Graham in WEIRD RANT</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Donald Trump went on a weird rant which visibly stunned Lindsey Graham and also threatened to hurt blue states and cities.</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2026-01-05T19:39:43Z</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>637</v>
+      </c>
+      <c r="F21" t="n">
+        <v>29394</v>
+      </c>
+      <c r="G21" t="n">
+        <v>341</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Pondering Politics</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=xged_Pzo35Q</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>简体中文</t>
+        </is>
+      </c>
+      <c r="L21" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>-3nzKAcEvxk</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Trump SINKS TO NEW LOW in DISGUSTING STUNT</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Donald Trump publicly mocks the brutal assassination of a Democratic lawmaker, whose children publicly beg him to stop.</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2026-01-05T18:34:22Z</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>626</v>
+      </c>
+      <c r="F22" t="n">
+        <v>65437</v>
+      </c>
+      <c r="G22" t="n">
+        <v>576</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Pondering Politics</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=-3nzKAcEvxk</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>简体中文</t>
+        </is>
+      </c>
+      <c r="L22" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Xj8JGZVgYFQ</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Marco Rubio ENDS CAREER by HUMILIATING Trump on LIVE TV</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Marco Rubio once again accidentally humiliated Donald Trump on live TV.</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2026-01-04T23:07:00Z</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>693</v>
+      </c>
+      <c r="F23" t="n">
+        <v>245636</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1773</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Pondering Politics</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=Xj8JGZVgYFQ</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>简体中文</t>
+        </is>
+      </c>
+      <c r="L23" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>4stBTanieHM</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>🚨 Trump THREATENS MORE WAR as Venezuela GIVES HIM THE FINGER</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>A furious Donald Trump publicly threatened to escalate his regime change war in Venezuela after the interim leader humiliated him.</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2026-01-04T19:07:00Z</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>619</v>
+      </c>
+      <c r="F24" t="n">
+        <v>53202</v>
+      </c>
+      <c r="G24" t="n">
+        <v>721</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Pondering Politics</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=4stBTanieHM</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>简体中文</t>
+        </is>
+      </c>
+      <c r="L24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>XUCBoQLmwyQ</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>🚨 BOMBSHELL: Rubio SCREWS Trump, ADMITS DEADLY VENEZUELA LEAK</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Marco Rubio confirms bombshell reporting that the Trump administration accidentally leaked sensitive war information about their Venezuela war to the press.</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2026-01-04T18:07:00Z</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>569</v>
+      </c>
+      <c r="F25" t="n">
+        <v>151417</v>
+      </c>
+      <c r="G25" t="n">
+        <v>953</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Pondering Politics</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=XUCBoQLmwyQ</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>简体中文</t>
+        </is>
+      </c>
+      <c r="L25" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>fLgZFbGt3KA</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>🚨 STUNNING: Venezuela HUMILIATES Trump on LIVE TV</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Venezuela's leadership, including interim president Delcy Rodriguez, publicly humiliated Donald Trump and rejected his claims they would roll over for him.</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>2026-01-03T21:09:12Z</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>632</v>
+      </c>
+      <c r="F26" t="n">
+        <v>687161</v>
+      </c>
+      <c r="G26" t="n">
+        <v>7457</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Pondering Politics</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=fLgZFbGt3KA</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>简体中文</t>
+        </is>
+      </c>
+      <c r="L26" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>FAn7bWn1uUM</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Will Trump Steal Greenland</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>In this video I talk about what happened on the 4th of January! The craziest is Trump wanting Greenland and honestly not something I expected!</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>2026-01-06T06:25:35Z</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>666</v>
+      </c>
+      <c r="F27" t="n">
+        <v>1452</v>
+      </c>
+      <c r="G27" t="n">
+        <v>88</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Omar Agamy</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=FAn7bWn1uUM</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>简体中文</t>
+        </is>
+      </c>
+      <c r="L27" t="n">
+        <v>0</v>
+      </c>
+      <c r="M27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>xCssF6vNGwU</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>What Trump Did To Venezuela</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>In this video I am talking about what the US did in Venezuela and how crazy the situation was in there. Honestly this story is enough to fill a whole day worth of videos cause it has been crazy,</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2026-01-05T04:57:58Z</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>483</v>
+      </c>
+      <c r="F28" t="n">
+        <v>9622</v>
+      </c>
+      <c r="G28" t="n">
+        <v>381</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Omar Agamy</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=xCssF6vNGwU</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>简体中文</t>
+        </is>
+      </c>
+      <c r="L28" t="n">
+        <v>0</v>
+      </c>
+      <c r="M28" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>